<commit_message>
adding selumetinib srb data
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Selumetinib_only/Selumetinib_SRB_data.xlsx
+++ b/Raw_SRB_data/Selumetinib_only/Selumetinib_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="S4" sheetId="5" r:id="rId4"/>
     <sheet name="S5" sheetId="1" r:id="rId5"/>
     <sheet name="S6" sheetId="6" r:id="rId6"/>
+    <sheet name="S7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -86,6 +87,12 @@
   </si>
   <si>
     <t>Passage #10</t>
+  </si>
+  <si>
+    <t>Passage #12</t>
+  </si>
+  <si>
+    <t>Day  1 date: 8/8/19</t>
   </si>
 </sst>
 </file>
@@ -3003,6 +3010,489 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="B7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D7">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E7">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.09</v>
+      </c>
+      <c r="G7">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="H7">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I7">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.107</v>
+      </c>
+      <c r="K7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L7">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.105</v>
+      </c>
+      <c r="B8">
+        <v>1.0629999999999999</v>
+      </c>
+      <c r="C8">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="D8">
+        <v>1.159</v>
+      </c>
+      <c r="E8">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F8">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="G8">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="H8">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.156</v>
+      </c>
+      <c r="J8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.107</v>
+      </c>
+      <c r="L8">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="B9">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="D9">
+        <v>1.077</v>
+      </c>
+      <c r="E9">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F9">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.106</v>
+      </c>
+      <c r="K9">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="L9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10">
+        <v>1.073</v>
+      </c>
+      <c r="C10">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.04</v>
+      </c>
+      <c r="E10">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G10">
+        <v>0.317</v>
+      </c>
+      <c r="H10">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="L10">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.376</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.191</v>
+      </c>
+      <c r="L11">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.995</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.006</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.184</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="L12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1.04</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.996</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.378</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="L13">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="B14">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E14">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F14">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G14">
+        <v>7.8E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.08</v>
+      </c>
+      <c r="I14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="J14">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K14">
+        <v>7.8E-2</v>
+      </c>
+      <c r="L14">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>AVERAGE(B11:B13)</f>
+        <v>1.0616666666666668</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:J16" si="0">AVERAGE(C11:C13)</f>
+        <v>0.99266666666666659</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.91</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.54966666666666664</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.37133333333333335</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.35933333333333328</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.19466666666666668</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE(K11:K13)</f>
+        <v>0.20333333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1.0616666666666668</v>
+      </c>
+      <c r="C18" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.99266666666666659</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19/1.061667*100</f>
+        <v>93.500755572761193</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0.91</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" ref="C20:C27" si="1">B20/1.061667*100</f>
+        <v>85.714258802430535</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="1"/>
+        <v>67.629492110049569</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.54966666666666664</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="1"/>
+        <v>51.773924089819758</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.37133333333333335</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="1"/>
+        <v>34.976441137695097</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.35933333333333328</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="1"/>
+        <v>33.846143219421279</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="1"/>
+        <v>26.687589737020488</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.19466666666666668</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="1"/>
+        <v>18.335944007552904</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.20333333333333334</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="1"/>
+        <v>19.152270281861767</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:C27"/>
     </sheetView>
@@ -3025,14 +3515,14 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3044,353 +3534,353 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8.7999999999999995E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="B7">
-        <v>7.6999999999999999E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="C7">
-        <v>8.4000000000000005E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="D7">
-        <v>8.2000000000000003E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E7">
-        <v>8.5999999999999993E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="F7">
-        <v>0.09</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G7">
-        <v>7.5999999999999998E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="H7">
-        <v>7.8E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="I7">
-        <v>7.1999999999999995E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J7">
-        <v>0.107</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="K7">
-        <v>6.9000000000000006E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L7">
-        <v>6.5000000000000002E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.105</v>
-      </c>
-      <c r="B8">
-        <v>1.0629999999999999</v>
-      </c>
-      <c r="C8">
-        <v>1.0940000000000001</v>
-      </c>
-      <c r="D8">
-        <v>1.159</v>
-      </c>
-      <c r="E8">
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="F8">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="G8">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="H8">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I8">
-        <v>0.156</v>
-      </c>
-      <c r="J8">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="K8">
-        <v>0.107</v>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.77</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.40300000000000002</v>
       </c>
       <c r="L8">
-        <v>0.10199999999999999</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9.4E-2</v>
-      </c>
-      <c r="B9">
-        <v>1.0449999999999999</v>
-      </c>
-      <c r="C9">
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="D9">
-        <v>1.077</v>
-      </c>
-      <c r="E9">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="F9">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="G9">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="H9">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="I9">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="J9">
-        <v>0.106</v>
-      </c>
-      <c r="K9">
-        <v>0.11799999999999999</v>
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.125</v>
       </c>
       <c r="L9">
-        <v>9.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.1</v>
-      </c>
-      <c r="B10">
-        <v>1.073</v>
-      </c>
-      <c r="C10">
-        <v>1.0509999999999999</v>
-      </c>
-      <c r="D10">
-        <v>1.04</v>
-      </c>
-      <c r="E10">
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="F10">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="G10">
-        <v>0.317</v>
-      </c>
-      <c r="H10">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="I10">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="J10">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="K10">
-        <v>0.11899999999999999</v>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.627</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.192</v>
       </c>
       <c r="L10">
-        <v>0.10100000000000001</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8.4000000000000005E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="B11" s="6">
-        <v>1.0860000000000001</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="C11" s="6">
-        <v>0.98699999999999999</v>
+        <v>0.43</v>
       </c>
       <c r="D11" s="6">
-        <v>0.83299999999999996</v>
+        <v>0.85199999999999998</v>
       </c>
       <c r="E11" s="6">
-        <v>0.65800000000000003</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="F11" s="6">
-        <v>0.58899999999999997</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="G11" s="6">
-        <v>0.44900000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="H11" s="6">
-        <v>0.376</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="I11" s="6">
-        <v>0.30599999999999999</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="J11" s="6">
-        <v>0.20300000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="K11" s="6">
-        <v>0.191</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="L11">
-        <v>0.106</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9.8000000000000004E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="B12" s="6">
-        <v>1.0589999999999999</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="C12" s="6">
-        <v>0.995</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="D12" s="6">
-        <v>1.006</v>
+        <v>0.83</v>
       </c>
       <c r="E12" s="6">
-        <v>0.83399999999999996</v>
+        <v>0.623</v>
       </c>
       <c r="F12" s="6">
-        <v>0.61099999999999999</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="G12" s="6">
-        <v>0.39900000000000002</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="H12" s="6">
-        <v>0.32400000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="I12" s="6">
-        <v>0.28100000000000003</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="J12" s="6">
-        <v>0.184</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="K12" s="6">
-        <v>0.17799999999999999</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="L12">
-        <v>9.8000000000000004E-2</v>
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1.04</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.996</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0.378</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="K13" s="6">
-        <v>0.24099999999999999</v>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="B13">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="C13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D13">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E13">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F13">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="G13">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="H13">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.08</v>
+      </c>
+      <c r="K13">
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="L13">
-        <v>7.8E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5.8000000000000003E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="B14">
-        <v>6.7000000000000004E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="C14">
-        <v>6.6000000000000003E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="D14">
-        <v>8.5999999999999993E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E14">
-        <v>7.4999999999999997E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F14">
-        <v>8.8999999999999996E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="G14">
-        <v>7.8E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H14">
-        <v>0.08</v>
+        <v>6.3E-2</v>
       </c>
       <c r="I14">
-        <v>8.1000000000000003E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="J14">
-        <v>6.4000000000000001E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="K14">
-        <v>7.8E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="L14">
-        <v>6.3E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16">
-        <f>AVERAGE(B11:B13)</f>
-        <v>1.0616666666666668</v>
+        <f>AVERAGE(B8:B12)</f>
+        <v>0.59800000000000009</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:K18" si="0">AVERAGE(C11:C13)</f>
-        <v>0.99266666666666659</v>
+        <f t="shared" ref="C16:K16" si="0">AVERAGE(C8:C12)</f>
+        <v>0.55940000000000012</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0.91</v>
+        <v>0.69940000000000002</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.71799999999999997</v>
+        <v>0.62899999999999989</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0.54966666666666664</v>
+        <v>0.55940000000000001</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>0.37133333333333335</v>
+        <v>0.42259999999999998</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0.35933333333333328</v>
+        <v>0.35200000000000004</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>0.28333333333333333</v>
+        <v>0.3024</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0.19466666666666668</v>
+        <v>0.24679999999999999</v>
       </c>
       <c r="K16">
-        <f>AVERAGE(K11:K13)</f>
-        <v>0.20333333333333334</v>
+        <f t="shared" si="0"/>
+        <v>0.21859999999999999</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>1.0616666666666668</v>
+        <v>0.59800000000000009</v>
       </c>
       <c r="C18" s="7">
         <v>100</v>
@@ -3398,83 +3888,83 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>0.99266666666666659</v>
+        <v>0.55940000000000012</v>
       </c>
       <c r="C19" s="7">
-        <f>B19/1.061667*100</f>
-        <v>93.500755572761193</v>
+        <f>B19/0.598*100</f>
+        <v>93.545150501672268</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>0.91</v>
+        <v>0.69940000000000002</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20:C27" si="1">B20/1.061667*100</f>
-        <v>85.714258802430535</v>
+        <f t="shared" ref="C20:C27" si="1">B20/0.598*100</f>
+        <v>116.95652173913045</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>0.71799999999999997</v>
+        <v>0.62899999999999989</v>
       </c>
       <c r="C21" s="7">
         <f t="shared" si="1"/>
-        <v>67.629492110049569</v>
+        <v>105.1839464882943</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>0.54966666666666664</v>
+        <v>0.55940000000000001</v>
       </c>
       <c r="C22" s="7">
         <f t="shared" si="1"/>
-        <v>51.773924089819758</v>
+        <v>93.545150501672254</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>0.37133333333333335</v>
+        <v>0.42259999999999998</v>
       </c>
       <c r="C23" s="7">
         <f t="shared" si="1"/>
-        <v>34.976441137695097</v>
+        <v>70.668896321070235</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>0.35933333333333328</v>
+        <v>0.35200000000000004</v>
       </c>
       <c r="C24" s="7">
         <f t="shared" si="1"/>
-        <v>33.846143219421279</v>
+        <v>58.862876254180605</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>0.28333333333333333</v>
+        <v>0.3024</v>
       </c>
       <c r="C25" s="7">
         <f t="shared" si="1"/>
-        <v>26.687589737020488</v>
+        <v>50.568561872909697</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>0.19466666666666668</v>
+        <v>0.24679999999999999</v>
       </c>
       <c r="C26" s="7">
         <f t="shared" si="1"/>
-        <v>18.335944007552904</v>
+        <v>41.270903010033443</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>0.20333333333333334</v>
+        <v>0.21859999999999999</v>
       </c>
       <c r="C27" s="7">
         <f t="shared" si="1"/>
-        <v>19.152270281861767</v>
+        <v>36.555183946488299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating last week's entries and protocols
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Selumetinib_only/Selumetinib_SRB_data.xlsx
+++ b/Raw_SRB_data/Selumetinib_only/Selumetinib_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="S5" sheetId="1" r:id="rId5"/>
     <sheet name="S6" sheetId="6" r:id="rId6"/>
     <sheet name="S7" sheetId="7" r:id="rId7"/>
+    <sheet name="S" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -93,6 +94,12 @@
   </si>
   <si>
     <t>Day  1 date: 8/8/19</t>
+  </si>
+  <si>
+    <t>Replicate # 7</t>
+  </si>
+  <si>
+    <t>Replicate # 8</t>
   </si>
 </sst>
 </file>
@@ -3493,8 +3500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3508,7 +3515,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3970,4 +3977,356 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="B8">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.113</v>
+      </c>
+      <c r="D8">
+        <v>0.104</v>
+      </c>
+      <c r="E8">
+        <v>0.106</v>
+      </c>
+      <c r="F8">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G8">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="I8">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="J8">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K8">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="B9">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.245</v>
+      </c>
+      <c r="D9">
+        <v>0.255</v>
+      </c>
+      <c r="E9">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="F9">
+        <v>0.67</v>
+      </c>
+      <c r="G9">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="H9">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.377</v>
+      </c>
+      <c r="J9">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.317</v>
+      </c>
+      <c r="L9">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="B10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.112</v>
+      </c>
+      <c r="D10">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="H10">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="I10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="J10">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="K10">
+        <v>0.315</v>
+      </c>
+      <c r="L10">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="B11">
+        <v>0.129</v>
+      </c>
+      <c r="C11">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E11">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G11">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H11">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="I11">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="J11">
+        <v>0.317</v>
+      </c>
+      <c r="K11">
+        <v>0.316</v>
+      </c>
+      <c r="L11">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="B12">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.154</v>
+      </c>
+      <c r="D12">
+        <v>0.182</v>
+      </c>
+      <c r="E12">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.23</v>
+      </c>
+      <c r="G12">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="I12">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="J12">
+        <v>0.32</v>
+      </c>
+      <c r="K12">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="L12">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="B13">
+        <v>0.246</v>
+      </c>
+      <c r="C13">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="E13">
+        <v>0.182</v>
+      </c>
+      <c r="F13">
+        <v>0.26</v>
+      </c>
+      <c r="G13">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="H13">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="I13">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="J13">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="K13">
+        <v>0.316</v>
+      </c>
+      <c r="L13">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.09</v>
+      </c>
+      <c r="B14">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="C14">
+        <v>0.104</v>
+      </c>
+      <c r="D14">
+        <v>0.115</v>
+      </c>
+      <c r="E14">
+        <v>0.104</v>
+      </c>
+      <c r="F14">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.111</v>
+      </c>
+      <c r="H14">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I14">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="J14">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="K14">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="L14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="B15">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="C15">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D15">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.09</v>
+      </c>
+      <c r="F15">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G15">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="I15">
+        <v>7.8E-2</v>
+      </c>
+      <c r="J15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K15">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L15">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating selumetinib objective summary
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Selumetinib_only/Selumetinib_SRB_data.xlsx
+++ b/Raw_SRB_data/Selumetinib_only/Selumetinib_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="S6" sheetId="6" r:id="rId6"/>
     <sheet name="S7" sheetId="7" r:id="rId7"/>
     <sheet name="S8" sheetId="8" r:id="rId8"/>
+    <sheet name="S9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -103,6 +104,15 @@
   </si>
   <si>
     <t>&lt;- not going to put in prism because of over enthusiastic plate shaking</t>
+  </si>
+  <si>
+    <t>Replicate # 9</t>
+  </si>
+  <si>
+    <t>Day  1 date: 22/8/19</t>
+  </si>
+  <si>
+    <t>Day  1 date: 12/8/19</t>
   </si>
 </sst>
 </file>
@@ -181,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -191,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3986,8 +3997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4008,7 +4019,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4335,7 +4346,7 @@
         <v>0.1552</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:K19" si="0">AVERAGE(C9:C13)</f>
+        <f t="shared" ref="C17:K17" si="0">AVERAGE(C9:C13)</f>
         <v>0.17760000000000001</v>
       </c>
       <c r="D17">
@@ -4461,6 +4472,489 @@
       <c r="C28" s="7">
         <f t="shared" si="1"/>
         <v>205.28350515463916</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.2E-2</v>
+      </c>
+      <c r="B7">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E7">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F7">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G7">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I7">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J7">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.109</v>
+      </c>
+      <c r="L7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1.359</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.23</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.2390000000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.018</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="L9">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.361</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.238</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.438</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="L10">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.874</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1.3160000000000001</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="L11">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1.341</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.2529999999999999</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="L12">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="B13">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C13">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D13">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="E13">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.161</v>
+      </c>
+      <c r="H13">
+        <v>0.123</v>
+      </c>
+      <c r="I13">
+        <v>9.4E-2</v>
+      </c>
+      <c r="J13">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="K13">
+        <v>0.08</v>
+      </c>
+      <c r="L13">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="B14">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C14">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D14">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F14">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G14">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I14">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="J14">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="K14">
+        <v>0.125</v>
+      </c>
+      <c r="L14">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>AVERAGE(B8:B12)</f>
+        <v>1.3328</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:K18" si="0">AVERAGE(C8:C12)</f>
+        <v>1.2154</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.101</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.93740000000000001</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.85599999999999987</v>
+      </c>
+      <c r="G16">
+        <f>AVERAGE(G8:G10,G12)</f>
+        <v>0.64175000000000004</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.43499999999999994</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0.32539999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1.3328</v>
+      </c>
+      <c r="C18" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1.2154</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19/1.3328*100</f>
+        <v>91.191476590636256</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.101</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" ref="C20:C27" si="1">B20/1.3328*100</f>
+        <v>82.608043217286919</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.93740000000000001</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="1"/>
+        <v>70.333133253301327</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.85599999999999987</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="1"/>
+        <v>64.225690276110441</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.64175000000000004</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="1"/>
+        <v>48.150510204081634</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="1"/>
+        <v>41.791716686674675</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.43499999999999994</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="1"/>
+        <v>32.63805522208883</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="1"/>
+        <v>23.229291716686674</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.32539999999999997</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="1"/>
+        <v>24.414765906362543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>